<commit_message>
some bug fixes, work on routing + query string for zini explorer/board editor
</commit_message>
<xml_diff>
--- a/src/assets/comparison.xlsx
+++ b/src/assets/comparison.xlsx
@@ -1,14 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harry\Desktop\Programming\Minesweeper stuff\llamasweeper\src\assets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1800BE6-676C-4913-BB74-C34629EC4FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E69550A-211E-47F3-88A0-8403BE135257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15705,5 +15700,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>